<commit_message>
ADD: pb-switch and wristband CAM files
</commit_message>
<xml_diff>
--- a/3. Design/7. PCB/pb-switch/output/pb-switch-bom.xlsx
+++ b/3. Design/7. PCB/pb-switch/output/pb-switch-bom.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repo\school\4th year\Project 1\Repository\zephyrus\3. Design\7. PCB\pb_switch\output\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repo\school\4th year\Project 1\Repository\zephyrus\3. Design\7. PCB\pb-switch\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83B94928-2414-48A3-BA1A-B65E0F4167F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDDDD25B-7BE1-4E10-AA69-2E81D6579CDE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8040" yWindow="5865" windowWidth="27930" windowHeight="11775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="1170" windowWidth="27930" windowHeight="11775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -717,7 +717,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -767,6 +767,12 @@
   </cellStyles>
   <dxfs count="17">
     <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1205,7 +1211,7 @@
   <dimension ref="A2:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>